<commit_message>
update logboek tot nu toe - jasper
</commit_message>
<xml_diff>
--- a/logboek_jasper.xlsx
+++ b/logboek_jasper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Challange_Week-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D73B8F0-30ED-4C74-9D01-49A40F100297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED587B48-C52F-41E1-8550-8DD386467802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{D8E002C3-334E-4C47-8488-F41D8686049C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D8E002C3-334E-4C47-8488-F41D8686049C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>datum</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>flush = True in de print zetten</t>
+  </si>
+  <si>
+    <t>comments, douane verhaal, winkel gefixed</t>
+  </si>
+  <si>
+    <t>random gate selectie</t>
+  </si>
+  <si>
+    <t>functie die een random variabele uit een lijst pakt met even kansen en die teruggeeft</t>
   </si>
 </sst>
 </file>
@@ -124,10 +133,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -443,52 +459,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932390AF-8C0A-4B7D-9BF6-078AB6555E27}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="4" width="36.7109375" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="36.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>45194</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>45185</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
logboek update, einde van de dag.
</commit_message>
<xml_diff>
--- a/logboek_jasper.xlsx
+++ b/logboek_jasper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Challange_Week-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED587B48-C52F-41E1-8550-8DD386467802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380648AE-5694-4865-8CC1-916737F6AE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D8E002C3-334E-4C47-8488-F41D8686049C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>datum</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>functie die een random variabele uit een lijst pakt met even kansen en die teruggeeft</t>
+  </si>
+  <si>
+    <t>meedere bestanden, twee extra locaties, nog meer aanpassingen aan de winkel</t>
+  </si>
+  <si>
+    <t>de verhalen dictionary werd te groot, de speler moet nog steeds sommige items kunnen krijgen ookal hoeft hij niet meer naar de winkel</t>
+  </si>
+  <si>
+    <t>verhalen naar een ander python bestand verplaatst, de speler kan kiezen om nog steeds naar de winkel te gaan</t>
   </si>
 </sst>
 </file>
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932390AF-8C0A-4B7D-9BF6-078AB6555E27}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,12 +517,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>45185</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -523,6 +532,23 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>45185</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>